<commit_message>
Add immigration data for 2022
</commit_message>
<xml_diff>
--- a/assignment3-population-dynamics/Population-Data.xlsx
+++ b/assignment3-population-dynamics/Population-Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenwong/school-work/active/math232-linear-algebra/assignment3-population-dynamics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B91EE99-2F87-B54B-ACF3-36D71D341B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3186AEFA-9DF1-4F92-BAEA-0297576983C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20940" activeTab="2" xr2:uid="{D43EF082-5E82-47AF-B540-29C22908F9BA}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{D43EF082-5E82-47AF-B540-29C22908F9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Age Distribution" sheetId="1" r:id="rId1"/>
     <sheet name="Birth Rate" sheetId="2" r:id="rId2"/>
     <sheet name="Mortality Rates" sheetId="3" r:id="rId3"/>
+    <sheet name="Immigration Rate" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Age</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>People</t>
+  </si>
+  <si>
+    <t>Persons</t>
   </si>
 </sst>
 </file>
@@ -407,19 +411,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B1754F-1237-43E2-B6C4-C32BA22DA1F9}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0">
-      <selection activeCell="F114" sqref="F114"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -427,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -435,7 +439,7 @@
         <v>376231</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -443,7 +447,7 @@
         <v>376231</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -451,7 +455,7 @@
         <v>376231</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -460,7 +464,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -469,7 +473,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -478,7 +482,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -487,7 +491,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -496,7 +500,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -505,7 +509,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -514,7 +518,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -523,7 +527,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -532,7 +536,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -541,7 +545,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -550,7 +554,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -559,7 +563,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -568,7 +572,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -577,7 +581,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -586,7 +590,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -595,7 +599,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -604,7 +608,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -614,7 +618,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -624,7 +628,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -634,7 +638,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -644,7 +648,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -654,7 +658,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -662,7 +666,7 @@
         <v>540744.19999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -670,7 +674,7 @@
         <v>540744.19999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -678,7 +682,7 @@
         <v>540744.19999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -686,7 +690,7 @@
         <v>540744.19999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -694,7 +698,7 @@
         <v>540744.19999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -702,7 +706,7 @@
         <v>556613</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -710,7 +714,7 @@
         <v>556613</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -718,7 +722,7 @@
         <v>556613</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -726,7 +730,7 @@
         <v>556613</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -734,7 +738,7 @@
         <v>556613</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -742,7 +746,7 @@
         <v>543783</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -750,7 +754,7 @@
         <v>543783</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -758,7 +762,7 @@
         <v>543783</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -766,7 +770,7 @@
         <v>543783</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -774,7 +778,7 @@
         <v>543783</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -782,7 +786,7 @@
         <v>514738.6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -790,7 +794,7 @@
         <v>514738.6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -798,7 +802,7 @@
         <v>514738.6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -806,7 +810,7 @@
         <v>514738.6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -814,7 +818,7 @@
         <v>514738.6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -822,7 +826,7 @@
         <v>481137.8</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -830,7 +834,7 @@
         <v>481137.8</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -838,7 +842,7 @@
         <v>481137.8</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -846,7 +850,7 @@
         <v>481137.8</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -854,7 +858,7 @@
         <v>481137.8</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -862,7 +866,7 @@
         <v>484733.8</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -870,7 +874,7 @@
         <v>484733.8</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -878,7 +882,7 @@
         <v>484733.8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -886,7 +890,7 @@
         <v>484733.8</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -894,7 +898,7 @@
         <v>484733.8</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -902,7 +906,7 @@
         <v>527027.80000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -910,7 +914,7 @@
         <v>527027.80000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -918,7 +922,7 @@
         <v>527027.80000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -926,7 +930,7 @@
         <v>527027.80000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -934,7 +938,7 @@
         <v>527027.80000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -942,7 +946,7 @@
         <v>527993</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -950,7 +954,7 @@
         <v>527993</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -958,7 +962,7 @@
         <v>527993</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -966,7 +970,7 @@
         <v>527993</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -974,7 +978,7 @@
         <v>527993</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -982,7 +986,7 @@
         <v>461608.2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -990,7 +994,7 @@
         <v>461608.2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>461608.2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -1006,7 +1010,7 @@
         <v>461608.2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>461608.2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>375972.4</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -1030,7 +1034,7 @@
         <v>375972.4</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -1038,7 +1042,7 @@
         <v>375972.4</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>375972.4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>375972.4</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -1062,7 +1066,7 @@
         <v>276336.40000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>276336.40000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>276336.40000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>276336.40000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>276336.40000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>80</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>175734.39999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>175734.39999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>175734.39999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -1126,7 +1130,7 @@
         <v>175734.39999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>175734.39999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>105984.6</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>105984.6</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>105984.6</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>105984.6</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>89</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>105984.6</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>52116.6</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>91</v>
       </c>
@@ -1190,7 +1194,7 @@
         <v>52116.6</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>52116.6</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>52116.6</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>94</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>52116.6</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>15532.6</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>15532.6</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>97</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>15532.6</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>98</v>
       </c>
@@ -1246,7 +1250,7 @@
         <v>15532.6</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -1265,9 +1269,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1283,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1299,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1307,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1315,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1323,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1331,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1347,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1379,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1387,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1395,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1403,7 +1407,7 @@
         <v>2.4500000000000004E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1411,7 +1415,7 @@
         <v>2.4500000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1419,7 +1423,7 @@
         <v>2.4500000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1427,7 +1431,7 @@
         <v>2.4500000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1435,7 +1439,7 @@
         <v>2.4500000000000004E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1443,7 +1447,7 @@
         <v>1.3550000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1451,7 +1455,7 @@
         <v>1.3550000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1459,7 +1463,7 @@
         <v>1.3550000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1467,7 +1471,7 @@
         <v>1.3550000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1475,7 +1479,7 @@
         <v>1.3550000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1483,7 +1487,7 @@
         <v>3.8350000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1491,7 +1495,7 @@
         <v>3.8350000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1499,7 +1503,7 @@
         <v>3.8350000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1507,7 +1511,7 @@
         <v>3.8350000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1515,7 +1519,7 @@
         <v>3.8350000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1523,7 +1527,7 @@
         <v>5.3200000000000004E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>5.3200000000000004E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1539,7 +1543,7 @@
         <v>5.3200000000000004E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1547,7 +1551,7 @@
         <v>5.3200000000000004E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1555,7 +1559,7 @@
         <v>5.3200000000000004E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1563,7 +1567,7 @@
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1571,7 +1575,7 @@
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1587,7 +1591,7 @@
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1595,7 +1599,7 @@
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1603,7 +1607,7 @@
         <v>6.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>6.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1619,7 +1623,7 @@
         <v>6.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1627,7 +1631,7 @@
         <v>6.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1635,7 +1639,7 @@
         <v>6.0999999999999995E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1643,7 +1647,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1651,7 +1655,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1659,7 +1663,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1667,7 +1671,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1675,7 +1679,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1683,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1691,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1699,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1715,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1723,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1731,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1739,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1747,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1755,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1763,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1787,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1795,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1811,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1827,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1843,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1875,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1899,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1915,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1923,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1947,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1955,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2003,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2019,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2027,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2043,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2051,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2059,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -2084,13 +2088,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F1344B-5420-4735-BDBF-A4A9F01AC476}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2106,7 +2110,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2114,7 +2118,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2130,7 +2134,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2138,7 +2142,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2154,7 +2158,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2162,7 +2166,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2170,7 +2174,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2178,7 +2182,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2186,7 +2190,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2194,7 +2198,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2202,7 +2206,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2210,7 +2214,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2218,7 +2222,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2226,7 +2230,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2234,7 +2238,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2242,7 +2246,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2250,7 +2254,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2258,7 +2262,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2266,7 +2270,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2274,7 +2278,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2282,7 +2286,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2290,7 +2294,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2298,7 +2302,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2306,7 +2310,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2314,7 +2318,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2322,7 +2326,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2330,7 +2334,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2338,7 +2342,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2354,7 +2358,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2362,7 +2366,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2370,7 +2374,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2378,7 +2382,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2386,7 +2390,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2394,7 +2398,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2402,7 +2406,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2410,7 +2414,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2418,7 +2422,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2426,7 +2430,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2434,7 +2438,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2442,7 +2446,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2450,7 +2454,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2458,7 +2462,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2466,7 +2470,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2474,7 +2478,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2482,7 +2486,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2490,7 +2494,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2498,7 +2502,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2506,7 +2510,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2514,7 +2518,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2538,7 +2542,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2546,7 +2550,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2562,7 +2566,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2570,7 +2574,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2578,7 +2582,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2586,7 +2590,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2594,7 +2598,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2602,7 +2606,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2610,7 +2614,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2618,7 +2622,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2626,7 +2630,7 @@
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2634,7 +2638,7 @@
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2642,7 +2646,7 @@
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2650,7 +2654,7 @@
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2658,7 +2662,7 @@
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2666,7 +2670,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2674,7 +2678,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2682,7 +2686,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2690,7 +2694,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2698,7 +2702,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2706,7 +2710,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2714,7 +2718,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2722,7 +2726,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2730,7 +2734,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2746,7 +2750,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2754,7 +2758,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2762,7 +2766,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2770,7 +2774,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2786,7 +2790,7 @@
         <v>9.2799999999999994E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2794,7 +2798,7 @@
         <v>9.2799999999999994E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2802,7 +2806,7 @@
         <v>9.2799999999999994E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2810,7 +2814,7 @@
         <v>9.2799999999999994E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>9.2799999999999994E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2826,7 +2830,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2834,7 +2838,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2842,7 +2846,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2850,7 +2854,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2882,7 +2886,7 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2890,12 +2894,835 @@
         <v>0.19719999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101">
         <v>0.19719999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2F5997-9F74-472E-8C86-FC6A25EE53C8}">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>4225.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4225.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4225.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4225.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4225.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6174.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6174.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>6174.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>6174.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>6174.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>4983.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>4983.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>4983.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>4983.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>4983.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>3857.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>3857.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>3857.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>3857.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>3857.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>13081.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>13081.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>13081.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>13081.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>13081.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>22930</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>22930</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>22930</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>22930</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>22930</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>15678.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>15678.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>15678.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>15678.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>15678.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>9967</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>9967</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>9967</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>9967</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>9967</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>6026.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>6026.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>6026.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>6026.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>6026.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>3502.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>3502.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>3502.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>3502.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>3502.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>2030.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>2030.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>2030.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>2030.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>2030.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>1555.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>1555.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>1555.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>1555.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>1555.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>1575.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>1575.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>1575.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>1575.6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>1575.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>1394.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>1394.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>1394.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>1394.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>1394.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>393.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>393.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>393.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>393.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>393.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>167.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>167.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>167.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>167.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>167.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>